<commit_message>
BOM revised, gerbers generated
</commit_message>
<xml_diff>
--- a/BOM/solar_harvester_v1.0_m1_Rev0.xlsx
+++ b/BOM/solar_harvester_v1.0_m1_Rev0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\std_folders\OneDrive\Документы\EAGLE\projects\solar_harvester_v1.0_m1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259064B7-5966-471E-9E83-263508EB31BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4307DE-655F-4598-8DEF-321A1843D50C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="183">
   <si>
     <t>#</t>
   </si>
@@ -218,18 +218,9 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>GRM035R60J475ME15D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Murata Electronics </t>
   </si>
   <si>
-    <t>81-GRM035R60J475ME5D</t>
-  </si>
-  <si>
     <t>595-TPS613221ADBVR</t>
   </si>
   <si>
@@ -260,15 +251,6 @@
     <t>MAX17040</t>
   </si>
   <si>
-    <t>GRM188R60J226MEA0D</t>
-  </si>
-  <si>
-    <t>CAP CER 22UF 6.3V X5R 1608</t>
-  </si>
-  <si>
-    <t>81-GRM188R60J226ME0D</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -359,9 +341,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 4.7uF 6.3volts *Derate Voltage/Temp 0603</t>
-  </si>
-  <si>
     <t xml:space="preserve">Taiyo Yuden </t>
   </si>
   <si>
@@ -389,18 +368,6 @@
     <t>Vishay / Dale</t>
   </si>
   <si>
-    <t xml:space="preserve">Yageo </t>
-  </si>
-  <si>
-    <t>PE0805FRF070R002L</t>
-  </si>
-  <si>
-    <t>Current Sense Resistors - SMD 0.002 Ohm 1% 100ppm</t>
-  </si>
-  <si>
-    <t>603-PE805FRF070R002L</t>
-  </si>
-  <si>
     <t>INA226AIDGSR</t>
   </si>
   <si>
@@ -527,27 +494,6 @@
     <t>JP1, JP4</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM21BR60J107ME15L </t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 100UF 6.3V 20% 0805</t>
-  </si>
-  <si>
-    <t>81-GRM21BR60J107ME5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walsin </t>
-  </si>
-  <si>
-    <t>0402X106M6R3CT</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10uF 20% 6.3 Volts 0402</t>
-  </si>
-  <si>
-    <t>791-0402X106M6R3CT</t>
-  </si>
-  <si>
     <t>KOA Speer</t>
   </si>
   <si>
@@ -603,6 +549,57 @@
   </si>
   <si>
     <t>Solar Harvester  v1.0_m1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F931A107KBA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tantalum Capacitors - Solid SMD 10V 100uF 10% 1211 ESR= 1.2 Ohms </t>
+  </si>
+  <si>
+    <t>647-F931A107KBA</t>
+  </si>
+  <si>
+    <t>ZRB15XR61A106ME01D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT</t>
+  </si>
+  <si>
+    <t>81-ZRB15XR61A106ME1D</t>
+  </si>
+  <si>
+    <t>GRM188R61A226ME15D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 22uF 10volts *Derate Voltage/Temp</t>
+  </si>
+  <si>
+    <t>81-GRM188R61A226ME5D</t>
+  </si>
+  <si>
+    <t>IRC / TT Electronics</t>
+  </si>
+  <si>
+    <t>LRCS0805-R56JT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Sense Resistors - SMD 0805 .56 Ohms 5% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">756-LRCS0805-R56JT5 </t>
+  </si>
+  <si>
+    <t>LMK105BBJ475MVLF</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 10V 4.7uF 20% X5R</t>
+  </si>
+  <si>
+    <t>963-LMK105BBJ475MVLF</t>
   </si>
 </sst>
 </file>
@@ -1604,50 +1601,50 @@
     <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="42" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2095,7 +2092,7 @@
   <dimension ref="A2:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B41"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -2121,7 +2118,7 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:15" ht="16.5">
-      <c r="B3" s="70"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2143,19 +2140,19 @@
         <v>36</v>
       </c>
       <c r="D4" s="64"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="68" t="s">
+      <c r="J4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="68"/>
+      <c r="K4" s="78"/>
       <c r="L4" s="48"/>
       <c r="M4" s="14"/>
       <c r="N4" s="43"/>
@@ -2168,15 +2165,15 @@
         <v>37</v>
       </c>
       <c r="D5" s="64"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="45"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="49"/>
       <c r="M5" s="14"/>
       <c r="N5" s="43"/>
@@ -2186,38 +2183,38 @@
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="80" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="65"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="25"/>
       <c r="H6" s="45"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="67"/>
+      <c r="K6" s="77"/>
       <c r="L6" s="48" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="1:15">
       <c r="B7" s="5"/>
-      <c r="C7" s="66"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="65"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="4"/>
       <c r="H7" s="45"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="67"/>
+      <c r="K7" s="77"/>
       <c r="L7" s="50">
         <v>2</v>
       </c>
@@ -2226,17 +2223,17 @@
     </row>
     <row r="8" spans="1:15">
       <c r="B8" s="5"/>
-      <c r="C8" s="66"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="65"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
       <c r="G8" s="25"/>
       <c r="H8" s="46"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="67"/>
+      <c r="K8" s="77"/>
       <c r="L8" s="51" t="s">
         <v>13</v>
       </c>
@@ -2245,17 +2242,17 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" s="15"/>
-      <c r="C9" s="66"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="65"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="76"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="16"/>
       <c r="H9" s="47"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="67"/>
+      <c r="K9" s="77"/>
       <c r="L9" s="50" t="s">
         <v>33</v>
       </c>
@@ -2271,15 +2268,15 @@
         <v>39</v>
       </c>
       <c r="D10" s="61"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="78"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
       <c r="G10" s="16"/>
       <c r="H10" s="45"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="67"/>
+      <c r="K10" s="77"/>
       <c r="L10" s="51" t="s">
         <v>26</v>
       </c>
@@ -2291,18 +2288,18 @@
         <v>17</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D11" s="63"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="80"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="16"/>
       <c r="H11" s="45"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="77"/>
       <c r="L11" s="51" t="s">
         <v>19</v>
       </c>
@@ -2374,20 +2371,20 @@
         <v>1</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D16" s="53">
         <v>2</v>
       </c>
       <c r="E16" s="53"/>
       <c r="F16" s="53" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H16" s="54" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="I16" s="53"/>
       <c r="J16" s="53" t="s">
@@ -2400,7 +2397,7 @@
         <v>54</v>
       </c>
       <c r="M16" s="53" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="N16" s="53"/>
       <c r="O16" s="33"/>
@@ -2411,20 +2408,20 @@
         <v>2</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D17" s="53">
         <v>1</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="53" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="G17" s="53" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="I17" s="53"/>
       <c r="J17" s="53" t="s">
@@ -2437,7 +2434,7 @@
         <v>54</v>
       </c>
       <c r="M17" s="53" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="N17" s="53"/>
     </row>
@@ -2447,7 +2444,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="52" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D18" s="53">
         <v>1</v>
@@ -2456,13 +2453,13 @@
         <v>0</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G18" s="53" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I18" s="53"/>
       <c r="J18" s="53" t="s">
@@ -2475,7 +2472,7 @@
         <v>54</v>
       </c>
       <c r="M18" s="53" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="N18" s="56"/>
     </row>
@@ -2485,22 +2482,22 @@
         <v>4</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D19" s="53">
         <v>1</v>
       </c>
       <c r="E19" s="53" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G19" s="53" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H19" s="54" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53" t="s">
@@ -2513,7 +2510,7 @@
         <v>54</v>
       </c>
       <c r="M19" s="53" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N19" s="53"/>
     </row>
@@ -2523,22 +2520,22 @@
         <v>5</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D20" s="53">
         <v>2</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G20" s="55" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H20" s="54" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53" t="s">
@@ -2551,7 +2548,7 @@
         <v>54</v>
       </c>
       <c r="M20" s="53" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="N20" s="53"/>
     </row>
@@ -2561,22 +2558,22 @@
         <v>6</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D21" s="53">
         <v>1</v>
       </c>
       <c r="E21" s="53" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="H21" s="54" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="I21" s="53"/>
       <c r="J21" s="53" t="s">
@@ -2589,7 +2586,7 @@
         <v>54</v>
       </c>
       <c r="M21" s="53" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="N21" s="53"/>
     </row>
@@ -2599,22 +2596,22 @@
         <v>7</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D22" s="53">
         <v>1</v>
       </c>
       <c r="E22" s="53" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F22" s="53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G22" s="53" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H22" s="54" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53" t="s">
@@ -2627,7 +2624,7 @@
         <v>54</v>
       </c>
       <c r="M22" s="53" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N22" s="53"/>
     </row>
@@ -2637,22 +2634,22 @@
         <v>8</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D23" s="53">
         <v>1</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="G23" s="53" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53" t="s">
@@ -2665,7 +2662,7 @@
         <v>54</v>
       </c>
       <c r="M23" s="53" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="N23" s="53"/>
     </row>
@@ -2675,22 +2672,22 @@
         <v>9</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D24" s="53">
         <v>1</v>
       </c>
       <c r="E24" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="53" t="s">
-        <v>108</v>
-      </c>
       <c r="H24" s="54" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53" t="s">
@@ -2703,7 +2700,7 @@
         <v>54</v>
       </c>
       <c r="M24" s="53" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N24" s="56"/>
     </row>
@@ -2713,22 +2710,22 @@
         <v>10</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D25" s="53">
         <v>1</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F25" s="53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G25" s="53" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="53" t="s">
@@ -2741,7 +2738,7 @@
         <v>54</v>
       </c>
       <c r="M25" s="53" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="N25" s="53"/>
     </row>
@@ -2751,22 +2748,22 @@
         <v>11</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D26" s="53">
         <v>2</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F26" s="53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G26" s="53" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="I26" s="53"/>
       <c r="J26" s="53" t="s">
@@ -2779,7 +2776,7 @@
         <v>54</v>
       </c>
       <c r="M26" s="53" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="N26" s="53"/>
     </row>
@@ -2789,22 +2786,22 @@
         <v>12</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D27" s="53">
         <v>1</v>
       </c>
       <c r="E27" s="53" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F27" s="53" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G27" s="53" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I27" s="53"/>
       <c r="J27" s="53" t="s">
@@ -2817,7 +2814,7 @@
         <v>54</v>
       </c>
       <c r="M27" s="53" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="N27" s="53"/>
     </row>
@@ -2833,16 +2830,16 @@
         <v>1</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F28" s="53" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="G28" s="53" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
       <c r="I28" s="53"/>
       <c r="J28" s="53" t="s">
@@ -2855,7 +2852,7 @@
         <v>54</v>
       </c>
       <c r="M28" s="53" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
       <c r="N28" s="53"/>
     </row>
@@ -2865,22 +2862,22 @@
         <v>14</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D29" s="53">
         <v>2</v>
       </c>
       <c r="E29" s="53" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F29" s="53" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G29" s="53" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
       <c r="H29" s="54" t="s">
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="I29" s="53"/>
       <c r="J29" s="53" t="s">
@@ -2893,7 +2890,7 @@
         <v>54</v>
       </c>
       <c r="M29" s="53" t="s">
-        <v>58</v>
+        <v>182</v>
       </c>
       <c r="N29" s="53"/>
     </row>
@@ -2909,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F30" s="53" t="s">
         <v>45</v>
@@ -2931,7 +2928,7 @@
         <v>54</v>
       </c>
       <c r="M30" s="53" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N30" s="53"/>
     </row>
@@ -2947,16 +2944,16 @@
         <v>1</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F31" s="53" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G31" s="53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H31" s="54" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I31" s="53"/>
       <c r="J31" s="53" t="s">
@@ -2969,7 +2966,7 @@
         <v>54</v>
       </c>
       <c r="M31" s="53" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N31" s="53"/>
     </row>
@@ -2979,22 +2976,22 @@
         <v>17</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D32" s="53">
         <v>1</v>
       </c>
       <c r="E32" s="53" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F32" s="53" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="H32" s="54" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="I32" s="53"/>
       <c r="J32" s="53" t="s">
@@ -3007,7 +3004,7 @@
         <v>54</v>
       </c>
       <c r="M32" s="53" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="N32" s="53"/>
     </row>
@@ -3017,22 +3014,22 @@
         <v>18</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D33" s="53">
         <v>4</v>
       </c>
       <c r="E33" s="53" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F33" s="53" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G33" s="53" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H33" s="54" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="I33" s="53"/>
       <c r="J33" s="53" t="s">
@@ -3045,7 +3042,7 @@
         <v>54</v>
       </c>
       <c r="M33" s="53" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="N33" s="53"/>
     </row>
@@ -3061,16 +3058,16 @@
         <v>1</v>
       </c>
       <c r="E34" s="53" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="F34" s="53" t="s">
         <v>41</v>
       </c>
       <c r="G34" s="53" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H34" s="54" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="I34" s="53"/>
       <c r="J34" s="53" t="s">
@@ -3083,7 +3080,7 @@
         <v>54</v>
       </c>
       <c r="M34" s="53" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="N34" s="53"/>
     </row>
@@ -3093,20 +3090,20 @@
         <v>20</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D35" s="53">
         <v>4</v>
       </c>
       <c r="E35" s="53"/>
       <c r="F35" s="53" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G35" s="53" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H35" s="54" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="I35" s="53"/>
       <c r="J35" s="53" t="s">
@@ -3119,7 +3116,7 @@
         <v>54</v>
       </c>
       <c r="M35" s="53" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="N35" s="53"/>
     </row>
@@ -3129,22 +3126,22 @@
         <v>21</v>
       </c>
       <c r="C36" s="52" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D36" s="53">
         <v>1</v>
       </c>
       <c r="E36" s="53" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F36" s="57" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="G36" s="57" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="H36" s="54" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="I36" s="53"/>
       <c r="J36" s="53" t="s">
@@ -3157,7 +3154,7 @@
         <v>54</v>
       </c>
       <c r="M36" s="53" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="N36" s="53"/>
     </row>
@@ -3167,25 +3164,25 @@
         <v>22</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D37" s="53">
         <v>1</v>
       </c>
       <c r="E37" s="53" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F37" s="53" t="s">
         <v>41</v>
       </c>
       <c r="G37" s="53" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H37" s="54" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="I37" s="53" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="J37" s="53" t="s">
         <v>30</v>
@@ -3197,7 +3194,7 @@
         <v>54</v>
       </c>
       <c r="M37" s="53" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="N37" s="53"/>
     </row>
@@ -3207,22 +3204,22 @@
         <v>23</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D38" s="53">
         <v>1</v>
       </c>
       <c r="E38" s="53" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F38" s="53" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="G38" s="53" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="H38" s="54" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="I38" s="53"/>
       <c r="J38" s="53" t="s">
@@ -3235,7 +3232,7 @@
         <v>54</v>
       </c>
       <c r="M38" s="53" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="N38" s="53"/>
     </row>
@@ -3245,25 +3242,25 @@
         <v>24</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D39" s="53">
         <v>1</v>
       </c>
       <c r="E39" s="53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F39" s="57" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G39" s="57" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H39" s="54" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="I39" s="53" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="J39" s="53" t="s">
         <v>30</v>
@@ -3275,7 +3272,7 @@
         <v>54</v>
       </c>
       <c r="M39" s="53" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="N39" s="53"/>
     </row>
@@ -3315,7 +3312,7 @@
         <v>54</v>
       </c>
       <c r="M40" s="53" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N40" s="53"/>
     </row>
@@ -3355,7 +3352,7 @@
         <v>54</v>
       </c>
       <c r="M41" s="53" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N41" s="42"/>
     </row>
@@ -3450,6 +3447,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C6:C9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J11:K11"/>
@@ -3458,7 +3456,6 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C6:C9"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" operator="equal" allowBlank="1" sqref="L7" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
increase comps sizes -> pcb reruting (in progress)
</commit_message>
<xml_diff>
--- a/BOM/solar_harvester_v1.0_m1_Rev0.xlsx
+++ b/BOM/solar_harvester_v1.0_m1_Rev0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\std_folders\OneDrive\Документы\EAGLE\projects\solar_harvester_v1.0_m1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4307DE-655F-4598-8DEF-321A1843D50C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B3BE4E-3C70-46A8-BF99-9D4BBB1D92CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -826,12 +826,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
@@ -1060,6 +1054,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1397,42 +1397,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1486,19 +1486,16 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="22" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="22" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1519,14 +1516,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1538,113 +1532,119 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="41" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="40" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="42" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="41" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="42" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="41" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="42" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="43" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2091,8 +2091,8 @@
   </sheetPr>
   <dimension ref="A2:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -2110,7 +2110,7 @@
     <col min="11" max="11" width="12.85546875" style="7" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.7109375" style="33" customWidth="1"/>
+    <col min="14" max="14" width="61.7109375" style="30" customWidth="1"/>
     <col min="15" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
@@ -2118,7 +2118,7 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:15" ht="16.5">
-      <c r="B3" s="66"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2130,181 +2130,181 @@
       <c r="K3" s="10"/>
       <c r="L3" s="11"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="44"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="1:15">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="41" t="s">
         <v>165</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="78" t="s">
+      <c r="J4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="48"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="44"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="43"/>
+      <c r="N4" s="39"/>
     </row>
     <row r="5" spans="1:15">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="45"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="49"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="45"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="43"/>
+      <c r="N5" s="39"/>
       <c r="O5" s="13"/>
     </row>
     <row r="6" spans="1:15" ht="42" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="45"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="77" t="s">
+      <c r="J6" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="77"/>
-      <c r="L6" s="48" t="s">
+      <c r="K6" s="74"/>
+      <c r="L6" s="44" t="s">
         <v>70</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="43"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:15">
       <c r="B7" s="5"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="45"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="77" t="s">
+      <c r="J7" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="77"/>
-      <c r="L7" s="50">
+      <c r="K7" s="74"/>
+      <c r="L7" s="46">
         <v>2</v>
       </c>
       <c r="M7" s="14"/>
-      <c r="N7" s="43"/>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:15">
       <c r="B8" s="5"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="46"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="77" t="s">
+      <c r="J8" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="77"/>
-      <c r="L8" s="51" t="s">
+      <c r="K8" s="74"/>
+      <c r="L8" s="47" t="s">
         <v>13</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="43"/>
+      <c r="N8" s="39"/>
     </row>
     <row r="9" spans="1:15">
       <c r="B9" s="15"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="68"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="47"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="77" t="s">
+      <c r="J9" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="77"/>
-      <c r="L9" s="50" t="s">
+      <c r="K9" s="74"/>
+      <c r="L9" s="46" t="s">
         <v>33</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9" s="43"/>
+      <c r="N9" s="39"/>
       <c r="O9" s="13"/>
     </row>
     <row r="10" spans="1:15">
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="45"/>
+      <c r="H10" s="41"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="77" t="s">
+      <c r="J10" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="77"/>
-      <c r="L10" s="51" t="s">
+      <c r="K10" s="74"/>
+      <c r="L10" s="47" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="14"/>
-      <c r="N10" s="43"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:15">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="45"/>
+      <c r="H11" s="41"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="77" t="s">
+      <c r="J11" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="77"/>
-      <c r="L11" s="51" t="s">
+      <c r="K11" s="74"/>
+      <c r="L11" s="47" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="14"/>
-      <c r="N11" s="43"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1">
       <c r="B12" s="3"/>
@@ -2319,7 +2319,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="43"/>
+      <c r="N12" s="39"/>
     </row>
     <row r="13" spans="1:15">
       <c r="N13" s="13"/>
@@ -2328,1122 +2328,1122 @@
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="58" t="s">
+      <c r="J15" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="58" t="s">
+      <c r="L15" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="60" t="s">
+      <c r="N15" s="56" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="32"/>
-      <c r="B16" s="34">
+      <c r="A16" s="29"/>
+      <c r="B16" s="31">
         <v>1</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="49">
         <v>2</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53" t="s">
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53" t="s">
+      <c r="I16" s="49"/>
+      <c r="J16" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="53">
+      <c r="K16" s="49">
         <v>3</v>
       </c>
-      <c r="L16" s="53" t="s">
+      <c r="L16" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="53" t="s">
+      <c r="M16" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="N16" s="53"/>
-      <c r="O16" s="33"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="30"/>
     </row>
     <row r="17" spans="1:14" ht="15">
-      <c r="A17" s="32"/>
-      <c r="B17" s="34">
+      <c r="A17" s="29"/>
+      <c r="B17" s="31">
         <v>2</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="49">
         <v>1</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53" t="s">
+      <c r="E17" s="49"/>
+      <c r="F17" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="53" t="s">
+      <c r="G17" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="H17" s="54" t="s">
+      <c r="H17" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53" t="s">
+      <c r="I17" s="49"/>
+      <c r="J17" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="53">
+      <c r="K17" s="49">
         <v>2</v>
       </c>
-      <c r="L17" s="53" t="s">
+      <c r="L17" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M17" s="53" t="s">
+      <c r="M17" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="N17" s="53"/>
+      <c r="N17" s="49"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
-      <c r="A18" s="32"/>
-      <c r="B18" s="42">
+      <c r="A18" s="29"/>
+      <c r="B18" s="38">
         <v>3</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="49">
         <v>1</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="49">
         <v>0</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="54" t="s">
+      <c r="H18" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53" t="s">
+      <c r="I18" s="49"/>
+      <c r="J18" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="53">
+      <c r="K18" s="49">
         <v>2</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="L18" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M18" s="53" t="s">
+      <c r="M18" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="56"/>
+      <c r="N18" s="52"/>
     </row>
     <row r="19" spans="1:14" ht="15">
-      <c r="A19" s="32"/>
-      <c r="B19" s="42">
+      <c r="A19" s="29"/>
+      <c r="B19" s="38">
         <v>4</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="49">
         <v>1</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="53" t="s">
+      <c r="G19" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53" t="s">
+      <c r="I19" s="49"/>
+      <c r="J19" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="53">
+      <c r="K19" s="49">
         <v>2</v>
       </c>
-      <c r="L19" s="53" t="s">
+      <c r="L19" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="53" t="s">
+      <c r="M19" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="N19" s="53"/>
+      <c r="N19" s="49"/>
     </row>
     <row r="20" spans="1:14" ht="15">
-      <c r="A20" s="32"/>
-      <c r="B20" s="42">
+      <c r="A20" s="29"/>
+      <c r="B20" s="38">
         <v>5</v>
       </c>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="49">
         <v>2</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="55" t="s">
+      <c r="G20" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53" t="s">
+      <c r="I20" s="49"/>
+      <c r="J20" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="53">
+      <c r="K20" s="49">
         <v>2</v>
       </c>
-      <c r="L20" s="53" t="s">
+      <c r="L20" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="53" t="s">
+      <c r="M20" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="53"/>
-    </row>
-    <row r="21" spans="1:14" s="28" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="42">
+      <c r="N20" s="49"/>
+    </row>
+    <row r="21" spans="1:14" s="25" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="38">
         <v>6</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="49">
         <v>1</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="53" t="s">
+      <c r="G21" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53" t="s">
+      <c r="I21" s="49"/>
+      <c r="J21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="53">
+      <c r="K21" s="49">
         <v>2</v>
       </c>
-      <c r="L21" s="53" t="s">
+      <c r="L21" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="53" t="s">
+      <c r="M21" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="N21" s="53"/>
+      <c r="N21" s="49"/>
     </row>
     <row r="22" spans="1:14" ht="15">
-      <c r="A22" s="32"/>
-      <c r="B22" s="42">
+      <c r="A22" s="29"/>
+      <c r="B22" s="38">
         <v>7</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="53">
+      <c r="D22" s="49">
         <v>1</v>
       </c>
-      <c r="E22" s="53" t="s">
+      <c r="E22" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="53" t="s">
+      <c r="F22" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53" t="s">
+      <c r="I22" s="49"/>
+      <c r="J22" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="53">
+      <c r="K22" s="49">
         <v>2</v>
       </c>
-      <c r="L22" s="53" t="s">
+      <c r="L22" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M22" s="53" t="s">
+      <c r="M22" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="N22" s="53"/>
+      <c r="N22" s="49"/>
     </row>
     <row r="23" spans="1:14" ht="15">
-      <c r="A23" s="32"/>
-      <c r="B23" s="42">
+      <c r="A23" s="29"/>
+      <c r="B23" s="38">
         <v>8</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="53">
+      <c r="D23" s="49">
         <v>1</v>
       </c>
-      <c r="E23" s="53" t="s">
+      <c r="E23" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="53" t="s">
+      <c r="G23" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53" t="s">
+      <c r="I23" s="49"/>
+      <c r="J23" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="53">
+      <c r="K23" s="49">
         <v>2</v>
       </c>
-      <c r="L23" s="53" t="s">
+      <c r="L23" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="53" t="s">
+      <c r="M23" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="N23" s="53"/>
+      <c r="N23" s="49"/>
     </row>
     <row r="24" spans="1:14" ht="15">
-      <c r="A24" s="32"/>
-      <c r="B24" s="42">
+      <c r="A24" s="29"/>
+      <c r="B24" s="38">
         <v>9</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="53">
+      <c r="D24" s="49">
         <v>1</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="53" t="s">
+      <c r="G24" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="H24" s="54" t="s">
+      <c r="H24" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53" t="s">
+      <c r="I24" s="49"/>
+      <c r="J24" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="53">
+      <c r="K24" s="49">
         <v>2</v>
       </c>
-      <c r="L24" s="53" t="s">
+      <c r="L24" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="53" t="s">
+      <c r="M24" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="N24" s="56"/>
+      <c r="N24" s="52"/>
     </row>
     <row r="25" spans="1:14" ht="15">
-      <c r="A25" s="32"/>
-      <c r="B25" s="42">
+      <c r="A25" s="29"/>
+      <c r="B25" s="38">
         <v>10</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="53">
+      <c r="D25" s="49">
         <v>1</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="53" t="s">
+      <c r="G25" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="54" t="s">
+      <c r="H25" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53" t="s">
+      <c r="I25" s="49"/>
+      <c r="J25" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="53">
+      <c r="K25" s="49">
         <v>2</v>
       </c>
-      <c r="L25" s="53" t="s">
+      <c r="L25" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="53" t="s">
+      <c r="M25" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="N25" s="53"/>
+      <c r="N25" s="49"/>
     </row>
     <row r="26" spans="1:14" ht="15">
-      <c r="A26" s="32"/>
-      <c r="B26" s="42">
+      <c r="A26" s="29"/>
+      <c r="B26" s="38">
         <v>11</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="53">
+      <c r="D26" s="49">
         <v>2</v>
       </c>
-      <c r="E26" s="53" t="s">
+      <c r="E26" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="53" t="s">
+      <c r="G26" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53" t="s">
+      <c r="I26" s="49"/>
+      <c r="J26" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K26" s="53">
+      <c r="K26" s="49">
         <v>2</v>
       </c>
-      <c r="L26" s="53" t="s">
+      <c r="L26" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M26" s="53" t="s">
+      <c r="M26" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="N26" s="53"/>
+      <c r="N26" s="49"/>
     </row>
     <row r="27" spans="1:14" ht="15">
-      <c r="A27" s="32"/>
-      <c r="B27" s="42">
+      <c r="A27" s="29"/>
+      <c r="B27" s="38">
         <v>12</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="53">
+      <c r="D27" s="49">
         <v>1</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="F27" s="53" t="s">
+      <c r="F27" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="G27" s="53" t="s">
+      <c r="G27" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="54" t="s">
+      <c r="H27" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53" t="s">
+      <c r="I27" s="49"/>
+      <c r="J27" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="53">
+      <c r="K27" s="49">
         <v>2</v>
       </c>
-      <c r="L27" s="53" t="s">
+      <c r="L27" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M27" s="53" t="s">
+      <c r="M27" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="N27" s="53"/>
-    </row>
-    <row r="28" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A28" s="32"/>
-      <c r="B28" s="42">
+      <c r="N27" s="49"/>
+    </row>
+    <row r="28" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A28" s="29"/>
+      <c r="B28" s="38">
         <v>13</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="49">
         <v>1</v>
       </c>
-      <c r="E28" s="53" t="s">
+      <c r="E28" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="53" t="s">
+      <c r="F28" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="G28" s="53" t="s">
+      <c r="G28" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="H28" s="54" t="s">
+      <c r="H28" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53" t="s">
+      <c r="I28" s="49"/>
+      <c r="J28" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="53">
+      <c r="K28" s="49">
         <v>2</v>
       </c>
-      <c r="L28" s="53" t="s">
+      <c r="L28" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M28" s="53" t="s">
+      <c r="M28" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="N28" s="53"/>
-    </row>
-    <row r="29" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A29" s="32"/>
-      <c r="B29" s="42">
+      <c r="N28" s="49"/>
+    </row>
+    <row r="29" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A29" s="29"/>
+      <c r="B29" s="38">
         <v>14</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="D29" s="53">
+      <c r="D29" s="49">
         <v>2</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E29" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="53" t="s">
+      <c r="F29" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="53" t="s">
+      <c r="G29" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="H29" s="54" t="s">
+      <c r="H29" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53" t="s">
+      <c r="I29" s="49"/>
+      <c r="J29" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="53">
+      <c r="K29" s="49">
         <v>2</v>
       </c>
-      <c r="L29" s="53" t="s">
+      <c r="L29" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M29" s="53" t="s">
+      <c r="M29" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="N29" s="53"/>
-    </row>
-    <row r="30" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A30" s="32"/>
-      <c r="B30" s="42">
+      <c r="N29" s="49"/>
+    </row>
+    <row r="30" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A30" s="29"/>
+      <c r="B30" s="38">
         <v>15</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="53">
+      <c r="D30" s="49">
         <v>1</v>
       </c>
-      <c r="E30" s="53" t="s">
+      <c r="E30" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="53" t="s">
+      <c r="F30" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="H30" s="54" t="s">
+      <c r="H30" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53" t="s">
+      <c r="I30" s="49"/>
+      <c r="J30" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="53">
+      <c r="K30" s="49">
         <v>2</v>
       </c>
-      <c r="L30" s="53" t="s">
+      <c r="L30" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M30" s="53" t="s">
+      <c r="M30" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="N30" s="53"/>
-    </row>
-    <row r="31" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A31" s="32"/>
-      <c r="B31" s="42">
+      <c r="N30" s="49"/>
+    </row>
+    <row r="31" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A31" s="29"/>
+      <c r="B31" s="38">
         <v>16</v>
       </c>
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="53">
+      <c r="D31" s="49">
         <v>1</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E31" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="53" t="s">
+      <c r="F31" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="53" t="s">
+      <c r="G31" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="H31" s="54" t="s">
+      <c r="H31" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53" t="s">
+      <c r="I31" s="49"/>
+      <c r="J31" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K31" s="53">
+      <c r="K31" s="49">
         <v>2</v>
       </c>
-      <c r="L31" s="53" t="s">
+      <c r="L31" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="53" t="s">
+      <c r="M31" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="N31" s="53"/>
+      <c r="N31" s="49"/>
     </row>
     <row r="32" spans="1:14" ht="15">
-      <c r="A32" s="32"/>
-      <c r="B32" s="42">
+      <c r="A32" s="29"/>
+      <c r="B32" s="38">
         <v>17</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D32" s="49">
         <v>1</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="H32" s="54" t="s">
+      <c r="H32" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53" t="s">
+      <c r="I32" s="49"/>
+      <c r="J32" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="53">
+      <c r="K32" s="49">
         <v>2</v>
       </c>
-      <c r="L32" s="53" t="s">
+      <c r="L32" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M32" s="53" t="s">
+      <c r="M32" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="N32" s="53"/>
+      <c r="N32" s="49"/>
     </row>
     <row r="33" spans="1:14" ht="15">
-      <c r="A33" s="32"/>
-      <c r="B33" s="42">
+      <c r="A33" s="29"/>
+      <c r="B33" s="38">
         <v>18</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="53">
+      <c r="D33" s="49">
         <v>4</v>
       </c>
-      <c r="E33" s="53" t="s">
+      <c r="E33" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="F33" s="53" t="s">
+      <c r="F33" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="53" t="s">
+      <c r="G33" s="49" t="s">
         <v>151</v>
       </c>
-      <c r="H33" s="54" t="s">
+      <c r="H33" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53" t="s">
+      <c r="I33" s="49"/>
+      <c r="J33" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="53">
+      <c r="K33" s="49">
         <v>2</v>
       </c>
-      <c r="L33" s="53" t="s">
+      <c r="L33" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M33" s="53" t="s">
+      <c r="M33" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="N33" s="53"/>
+      <c r="N33" s="49"/>
     </row>
     <row r="34" spans="1:14" ht="15">
-      <c r="A34" s="32"/>
-      <c r="B34" s="42">
+      <c r="A34" s="29"/>
+      <c r="B34" s="38">
         <v>19</v>
       </c>
-      <c r="C34" s="52" t="s">
+      <c r="C34" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="53">
+      <c r="D34" s="49">
         <v>1</v>
       </c>
-      <c r="E34" s="53" t="s">
+      <c r="E34" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="F34" s="53" t="s">
+      <c r="F34" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="53" t="s">
+      <c r="G34" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="H34" s="54" t="s">
+      <c r="H34" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53" t="s">
+      <c r="I34" s="49"/>
+      <c r="J34" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K34" s="53">
+      <c r="K34" s="49">
         <v>21</v>
       </c>
-      <c r="L34" s="53" t="s">
+      <c r="L34" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M34" s="53" t="s">
+      <c r="M34" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="N34" s="53"/>
-    </row>
-    <row r="35" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A35" s="32"/>
-      <c r="B35" s="42">
+      <c r="N34" s="49"/>
+    </row>
+    <row r="35" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A35" s="29"/>
+      <c r="B35" s="38">
         <v>20</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="53">
+      <c r="D35" s="49">
         <v>4</v>
       </c>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53" t="s">
+      <c r="E35" s="49"/>
+      <c r="F35" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="G35" s="53" t="s">
+      <c r="G35" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H35" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53" t="s">
+      <c r="I35" s="49"/>
+      <c r="J35" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K35" s="53">
+      <c r="K35" s="49">
         <v>2</v>
       </c>
-      <c r="L35" s="53" t="s">
+      <c r="L35" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M35" s="53" t="s">
+      <c r="M35" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="53"/>
-    </row>
-    <row r="36" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A36" s="32"/>
-      <c r="B36" s="42">
+      <c r="N35" s="49"/>
+    </row>
+    <row r="36" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A36" s="29"/>
+      <c r="B36" s="38">
         <v>21</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D36" s="49">
         <v>1</v>
       </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="57" t="s">
+      <c r="F36" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="G36" s="57" t="s">
+      <c r="G36" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53" t="s">
+      <c r="I36" s="49"/>
+      <c r="J36" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K36" s="53">
+      <c r="K36" s="49">
         <v>8</v>
       </c>
-      <c r="L36" s="53" t="s">
+      <c r="L36" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M36" s="53" t="s">
+      <c r="M36" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="N36" s="53"/>
+      <c r="N36" s="49"/>
     </row>
     <row r="37" spans="1:14" ht="15">
-      <c r="A37" s="32"/>
-      <c r="B37" s="42">
+      <c r="A37" s="29"/>
+      <c r="B37" s="38">
         <v>22</v>
       </c>
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="53">
+      <c r="D37" s="49">
         <v>1</v>
       </c>
-      <c r="E37" s="53" t="s">
+      <c r="E37" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="53" t="s">
+      <c r="F37" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G37" s="53" t="s">
+      <c r="G37" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H37" s="54" t="s">
+      <c r="H37" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="I37" s="53" t="s">
+      <c r="I37" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="J37" s="53" t="s">
+      <c r="J37" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K37" s="53">
+      <c r="K37" s="49">
         <v>10</v>
       </c>
-      <c r="L37" s="53" t="s">
+      <c r="L37" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M37" s="53" t="s">
+      <c r="M37" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="N37" s="53"/>
+      <c r="N37" s="49"/>
     </row>
     <row r="38" spans="1:14" ht="15">
-      <c r="A38" s="32"/>
-      <c r="B38" s="42">
+      <c r="A38" s="29"/>
+      <c r="B38" s="38">
         <v>23</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="53">
+      <c r="D38" s="49">
         <v>1</v>
       </c>
-      <c r="E38" s="53" t="s">
+      <c r="E38" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="F38" s="53" t="s">
+      <c r="F38" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="H38" s="54" t="s">
+      <c r="H38" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53" t="s">
+      <c r="I38" s="49"/>
+      <c r="J38" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K38" s="53">
+      <c r="K38" s="49">
         <v>2</v>
       </c>
-      <c r="L38" s="53" t="s">
+      <c r="L38" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M38" s="53" t="s">
+      <c r="M38" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="N38" s="53"/>
+      <c r="N38" s="49"/>
     </row>
     <row r="39" spans="1:14" ht="15">
-      <c r="A39" s="32"/>
-      <c r="B39" s="42">
+      <c r="A39" s="29"/>
+      <c r="B39" s="38">
         <v>24</v>
       </c>
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="53">
+      <c r="D39" s="49">
         <v>1</v>
       </c>
-      <c r="E39" s="53" t="s">
+      <c r="E39" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="57" t="s">
+      <c r="F39" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="57" t="s">
+      <c r="G39" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="H39" s="54" t="s">
+      <c r="H39" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="I39" s="53" t="s">
+      <c r="I39" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="J39" s="53" t="s">
+      <c r="J39" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K39" s="53">
+      <c r="K39" s="49">
         <v>9</v>
       </c>
-      <c r="L39" s="53" t="s">
+      <c r="L39" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="53" t="s">
+      <c r="M39" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="N39" s="53"/>
-    </row>
-    <row r="40" spans="1:14" s="33" customFormat="1" ht="15">
-      <c r="A40" s="32"/>
-      <c r="B40" s="42">
+      <c r="N39" s="49"/>
+    </row>
+    <row r="40" spans="1:14" s="30" customFormat="1" ht="15">
+      <c r="A40" s="29"/>
+      <c r="B40" s="38">
         <v>25</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="53">
+      <c r="D40" s="49">
         <v>1</v>
       </c>
-      <c r="E40" s="53" t="s">
+      <c r="E40" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="53" t="s">
+      <c r="F40" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="53" t="s">
+      <c r="G40" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H40" s="54" t="s">
+      <c r="H40" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I40" s="53" t="s">
+      <c r="I40" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="J40" s="53" t="s">
+      <c r="J40" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K40" s="53">
+      <c r="K40" s="49">
         <v>5</v>
       </c>
-      <c r="L40" s="53" t="s">
+      <c r="L40" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M40" s="53" t="s">
+      <c r="M40" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="N40" s="53"/>
-    </row>
-    <row r="41" spans="1:14" s="33" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="42">
+      <c r="N40" s="49"/>
+    </row>
+    <row r="41" spans="1:14" s="30" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A41" s="29"/>
+      <c r="B41" s="38">
         <v>26</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="53">
+      <c r="D41" s="49">
         <v>1</v>
       </c>
-      <c r="E41" s="53" t="s">
+      <c r="E41" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="53" t="s">
+      <c r="F41" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="53" t="s">
+      <c r="G41" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H41" s="54" t="s">
+      <c r="H41" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="53" t="s">
+      <c r="I41" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="J41" s="53" t="s">
+      <c r="J41" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K41" s="53">
+      <c r="K41" s="49">
         <v>5</v>
       </c>
-      <c r="L41" s="53" t="s">
+      <c r="L41" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="M41" s="53" t="s">
+      <c r="M41" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="N41" s="42"/>
+      <c r="N41" s="38"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A42" s="30"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="21">
         <f>COUNT(B16:B41)</f>
         <v>26</v>
       </c>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A43" s="30"/>
-      <c r="I43" s="26" t="s">
+      <c r="A43" s="27"/>
+      <c r="I43" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J43" s="27">
+      <c r="J43" s="24">
         <f>SUMPRODUCT(D16:D41,(J16:J41="THT")*1)</f>
         <v>7</v>
       </c>
-      <c r="K43" s="27">
+      <c r="K43" s="24">
         <f>SUMPRODUCT(D16:D41,K16:K41,(J16:J41="THT")*1)</f>
         <v>16</v>
       </c>
-      <c r="L43" s="37"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="36"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A44" s="30"/>
-      <c r="F44" s="22" t="s">
+      <c r="A44" s="27"/>
+      <c r="F44" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="23"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="26" t="s">
+      <c r="G44" s="78"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J44" s="38">
+      <c r="J44" s="35">
         <f>SUMPRODUCT(D16:D41,(J16:J41="SMD")*1)</f>
         <v>29</v>
       </c>
-      <c r="K44" s="38">
+      <c r="K44" s="35">
         <f>SUMPRODUCT(D16:D41,K16:K41,(J16:J41="SMD")*1)</f>
         <v>104</v>
       </c>
-      <c r="L44" s="35"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A45" s="30"/>
-      <c r="I45" s="26" t="s">
+      <c r="A45" s="27"/>
+      <c r="I45" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J45" s="39">
+      <c r="J45" s="80">
         <f>J43+J44</f>
         <v>36</v>
       </c>
-      <c r="K45" s="39">
+      <c r="K45" s="80">
         <f>K43+K44</f>
         <v>120</v>
       </c>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="30"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-    </row>
-    <row r="47" spans="1:14" s="30" customFormat="1">
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
+      <c r="A46" s="27"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+    </row>
+    <row r="47" spans="1:14" s="27" customFormat="1">
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="30"/>
+      <c r="A48" s="27"/>
     </row>
     <row r="56" spans="10:10" ht="15">
-      <c r="J56" s="29"/>
+      <c r="J56" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>